<commit_message>
LVGL port done, UART_CLI: 80%
</commit_message>
<xml_diff>
--- a/Hardware/Freezer_Controller/Fabrication files/Freezer_Controller_BOM.xlsx
+++ b/Hardware/Freezer_Controller/Fabrication files/Freezer_Controller_BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\3. Workplace\Altium\08.09. Freezer\Freezer_FW\Hardware\Freezer_Controller\Project Outputs for Freezer_Controller\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\3. Workplace\Altium\08.09. Freezer\_git\Freezer_FW\Hardware\Freezer_Controller\Fabrication files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D265B8A-3A92-43DD-800C-180CDA582962}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D02BCEE-7667-43E2-880A-609D9C905B9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7770" yWindow="4080" windowWidth="17145" windowHeight="11520" xr2:uid="{B333C20D-DB3D-49B3-B344-87822F657418}"/>
+    <workbookView xWindow="4800" yWindow="4050" windowWidth="15045" windowHeight="11520" xr2:uid="{B333C20D-DB3D-49B3-B344-87822F657418}"/>
   </bookViews>
   <sheets>
     <sheet name="Freezer_Controller" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="227">
   <si>
     <t>LibRef</t>
   </si>
@@ -696,13 +696,19 @@
     <t>R132</t>
   </si>
   <si>
-    <t>R22, R23, R26, R29, R128, R129, R130, R131</t>
-  </si>
-  <si>
     <t>A119933TR-ND</t>
   </si>
   <si>
     <t>311-10KDTR-ND</t>
+  </si>
+  <si>
+    <t>R22, R23, R26, R130, R131</t>
+  </si>
+  <si>
+    <t>R29, R128, R129</t>
+  </si>
+  <si>
+    <t>TNPW040210K0BEED</t>
   </si>
 </sst>
 </file>
@@ -1079,10 +1085,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B750D07F-CACC-46D7-8B96-1343A2CA061E}">
-  <dimension ref="A1:E74"/>
+  <dimension ref="A1:E75"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="C35" workbookViewId="0">
+      <selection activeCell="F46" sqref="F46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1860,31 +1866,29 @@
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="2" t="s">
-        <v>138</v>
-      </c>
+      <c r="A46" s="2"/>
       <c r="B46" s="2" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C46" s="1">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="D46" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>220</v>
+        <v>138</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="C47" s="1">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="D47" s="2" t="s">
         <v>7</v>
@@ -1895,10 +1899,10 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>139</v>
+        <v>220</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>140</v>
+        <v>221</v>
       </c>
       <c r="C48" s="1">
         <v>1</v>
@@ -1907,15 +1911,15 @@
         <v>7</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>141</v>
+        <v>222</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="C49" s="1">
         <v>1</v>
@@ -1924,66 +1928,66 @@
         <v>7</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C50" s="1">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D50" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="C51" s="1">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D51" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C52" s="1">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D52" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C53" s="1">
         <v>12</v>
@@ -1992,49 +1996,49 @@
         <v>7</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C54" s="1">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D54" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="C55" s="1">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D55" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="C56" s="1">
         <v>4</v>
@@ -2043,66 +2047,66 @@
         <v>7</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="C57" s="1">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D57" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="C58" s="1">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="D58" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="C59" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D59" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="C60" s="1">
         <v>1</v>
@@ -2111,49 +2115,49 @@
         <v>7</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="C61" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D61" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="C62" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D62" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="C63" s="1">
         <v>1</v>
@@ -2162,15 +2166,15 @@
         <v>7</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="C64" s="1">
         <v>1</v>
@@ -2179,15 +2183,15 @@
         <v>7</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="C65" s="1">
         <v>1</v>
@@ -2196,15 +2200,15 @@
         <v>7</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="C66" s="1">
         <v>1</v>
@@ -2213,66 +2217,66 @@
         <v>7</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="C67" s="1">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="D67" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C68" s="1">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D68" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="C69" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D69" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="C70" s="1">
         <v>1</v>
@@ -2281,15 +2285,15 @@
         <v>7</v>
       </c>
       <c r="E70" s="2" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="C71" s="1">
         <v>1</v>
@@ -2298,15 +2302,15 @@
         <v>7</v>
       </c>
       <c r="E71" s="2" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="C72" s="1">
         <v>1</v>
@@ -2315,15 +2319,15 @@
         <v>7</v>
       </c>
       <c r="E72" s="2" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="C73" s="1">
         <v>1</v>
@@ -2332,23 +2336,40 @@
         <v>7</v>
       </c>
       <c r="E73" s="2" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="C74" s="1">
+        <v>1</v>
+      </c>
+      <c r="D74" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E74" s="2" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75" s="2" t="s">
         <v>217</v>
       </c>
-      <c r="B74" s="2" t="s">
+      <c r="B75" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="C74" s="1">
-        <v>1</v>
-      </c>
-      <c r="D74" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E74" s="2" t="s">
+      <c r="C75" s="1">
+        <v>1</v>
+      </c>
+      <c r="D75" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E75" s="2" t="s">
         <v>219</v>
       </c>
     </row>

</xml_diff>